<commit_message>
praktik wait, verifikasi expected elemen, dan test suite
</commit_message>
<xml_diff>
--- a/dataFile.xlsx
+++ b/dataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="5664" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="5664"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>locatorItem</t>
+  </si>
+  <si>
+    <t>ddddd</t>
+  </si>
+  <si>
+    <t>cccccc</t>
   </si>
 </sst>
 </file>
@@ -390,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,6 +463,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -467,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>